<commit_message>
oublie APS dans report PS
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/Report PS.xlsx
+++ b/lib/PHPExcel/templates/Report PS.xlsx
@@ -763,7 +763,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
@@ -938,9 +938,6 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
@@ -1504,20 +1501,20 @@
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
       <c r="H7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1530,20 +1527,20 @@
       <c r="B8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
       <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
       <c r="H9" s="11" t="s">
         <v>10</v>
       </c>
@@ -1901,7 +1898,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B47" sqref="B47"/>
+      <selection pane="topRight" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2002,19 +1999,19 @@
     </row>
     <row r="14" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="36"/>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="69" t="s">
         <v>74</v>
       </c>
       <c r="D14" s="40"/>
-      <c r="E14" s="72"/>
+      <c r="E14" s="71"/>
     </row>
     <row r="15" spans="2:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="60"/>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="70" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="42"/>
-      <c r="E15" s="73"/>
+      <c r="E15" s="72"/>
     </row>
     <row r="16" spans="2:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="61" t="s">
@@ -2032,7 +2029,7 @@
       <c r="D17" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="74"/>
+      <c r="E17" s="73"/>
     </row>
     <row r="18" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="36" t="s">
@@ -2042,7 +2039,7 @@
       <c r="D18" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="74"/>
+      <c r="E18" s="73"/>
     </row>
     <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="36" t="s">
@@ -2052,7 +2049,7 @@
       <c r="D19" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="74"/>
+      <c r="E19" s="73"/>
     </row>
     <row r="20" spans="1:5" ht="14.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="43" t="s">
@@ -2072,7 +2069,7 @@
       <c r="D21" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="74"/>
+      <c r="E21" s="73"/>
     </row>
     <row r="22" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="43" t="s">
@@ -2080,7 +2077,7 @@
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="41"/>
-      <c r="E22" s="74"/>
+      <c r="E22" s="73"/>
     </row>
     <row r="23" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="36" t="s">
@@ -2090,7 +2087,7 @@
       <c r="D23" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="74"/>
+      <c r="E23" s="73"/>
     </row>
     <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="43" t="s">
@@ -2110,184 +2107,184 @@
       <c r="D25" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="74"/>
+      <c r="E25" s="73"/>
     </row>
     <row r="26" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="91"/>
-      <c r="D26" s="92" t="s">
+      <c r="C26" s="90"/>
+      <c r="D26" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="89"/>
+      <c r="E26" s="88"/>
     </row>
     <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="82" t="s">
+      <c r="B27" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="83" t="s">
+      <c r="C27" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="84" t="s">
+      <c r="D27" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="85"/>
+      <c r="E27" s="84"/>
     </row>
     <row r="28" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="95"/>
+      <c r="A28" s="94"/>
       <c r="B28" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="81" t="s">
+      <c r="D28" s="80" t="s">
         <v>26</v>
       </c>
       <c r="E28" s="51"/>
     </row>
     <row r="29" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="95"/>
-      <c r="B29" s="79" t="s">
+      <c r="A29" s="94"/>
+      <c r="B29" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="80" t="s">
+      <c r="C29" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="81" t="s">
+      <c r="D29" s="80" t="s">
         <v>79</v>
       </c>
       <c r="E29" s="52"/>
     </row>
     <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="95"/>
-      <c r="B30" s="79" t="s">
+      <c r="A30" s="94"/>
+      <c r="B30" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="80" t="s">
+      <c r="C30" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="81" t="s">
+      <c r="D30" s="80" t="s">
         <v>79</v>
       </c>
       <c r="E30" s="52"/>
     </row>
     <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="95"/>
-      <c r="B31" s="79" t="s">
+      <c r="A31" s="94"/>
+      <c r="B31" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="80"/>
-      <c r="D31" s="81" t="s">
+      <c r="C31" s="79"/>
+      <c r="D31" s="80" t="s">
         <v>79</v>
       </c>
       <c r="E31" s="52"/>
     </row>
     <row r="32" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="95"/>
-      <c r="B32" s="79" t="s">
+      <c r="A32" s="94"/>
+      <c r="B32" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="80"/>
-      <c r="D32" s="81"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="80"/>
       <c r="E32" s="52"/>
     </row>
     <row r="33" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="96"/>
-      <c r="B33" s="88" t="s">
+      <c r="A33" s="95"/>
+      <c r="B33" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="86"/>
-      <c r="D33" s="87" t="s">
+      <c r="C33" s="85"/>
+      <c r="D33" s="86" t="s">
         <v>19</v>
       </c>
       <c r="E33" s="59"/>
     </row>
     <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="94" t="s">
+      <c r="A34" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="82" t="s">
+      <c r="B34" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="83" t="s">
+      <c r="C34" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="84" t="s">
+      <c r="D34" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="85"/>
+      <c r="E34" s="84"/>
     </row>
     <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="95"/>
+      <c r="A35" s="94"/>
       <c r="B35" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="80" t="s">
+      <c r="C35" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="81" t="s">
+      <c r="D35" s="80" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="51"/>
     </row>
     <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="95"/>
-      <c r="B36" s="79" t="s">
+      <c r="A36" s="94"/>
+      <c r="B36" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="80" t="s">
+      <c r="C36" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="81" t="s">
+      <c r="D36" s="80" t="s">
         <v>79</v>
       </c>
       <c r="E36" s="52"/>
     </row>
     <row r="37" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="95"/>
-      <c r="B37" s="79" t="s">
+      <c r="A37" s="94"/>
+      <c r="B37" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="80" t="s">
+      <c r="C37" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="81" t="s">
+      <c r="D37" s="80" t="s">
         <v>79</v>
       </c>
       <c r="E37" s="52"/>
     </row>
     <row r="38" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="95"/>
-      <c r="B38" s="79" t="s">
+      <c r="A38" s="94"/>
+      <c r="B38" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="80"/>
-      <c r="D38" s="81" t="s">
+      <c r="C38" s="79"/>
+      <c r="D38" s="80" t="s">
         <v>79</v>
       </c>
       <c r="E38" s="52"/>
     </row>
     <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="95"/>
-      <c r="B39" s="79" t="s">
+      <c r="A39" s="94"/>
+      <c r="B39" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="80"/>
-      <c r="D39" s="81"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="80"/>
       <c r="E39" s="52"/>
     </row>
     <row r="40" spans="1:5" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="96"/>
-      <c r="B40" s="88" t="s">
+      <c r="A40" s="95"/>
+      <c r="B40" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="86"/>
-      <c r="D40" s="87" t="s">
+      <c r="C40" s="85"/>
+      <c r="D40" s="86" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="59"/>
@@ -2334,13 +2331,13 @@
       </c>
       <c r="C47" s="37"/>
       <c r="D47" s="40"/>
-      <c r="E47" s="69"/>
+      <c r="E47" s="55"/>
     </row>
     <row r="48" spans="1:5" s="19" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="75"/>
-      <c r="C48" s="76"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="78"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="75"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="77"/>
     </row>
     <row r="49" spans="2:104" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D49" s="44"/>
@@ -2544,29 +2541,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Check xmlns="67604082-326d-4240-aaee-100283b20839">Rapport Validé</Check>
-    <vctj xmlns="67604082-326d-4240-aaee-100283b20839">8043</vctj>
-    <pv7j xmlns="67604082-326d-4240-aaee-100283b20839">13232</pv7j>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006A18800F7AB66843AE086E8500CCEA21" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5d60d5c9f17a480d7e4b53ebba2c4603">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="67604082-326d-4240-aaee-100283b20839" xmlns:ns3="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b97804bffc58ba73e5228c2548755f2" ns2:_="" ns3:_="">
     <xsd:import namespace="67604082-326d-4240-aaee-100283b20839"/>
@@ -2742,40 +2716,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07ED7936-D779-47E7-BF6C-7C086F04E976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="67604082-326d-4240-aaee-100283b20839"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3C53B3C-BBC9-48C3-9DA4-3687FEE00EE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39F1329F-71F7-4F0E-A822-5837ADF5B51C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Check xmlns="67604082-326d-4240-aaee-100283b20839">Rapport Validé</Check>
+    <vctj xmlns="67604082-326d-4240-aaee-100283b20839">8043</vctj>
+    <pv7j xmlns="67604082-326d-4240-aaee-100283b20839">13232</pv7j>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{386C40D6-9904-47D7-9FC5-798E8189EC7C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2792,4 +2756,37 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39F1329F-71F7-4F0E-A822-5837ADF5B51C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3C53B3C-BBC9-48C3-9DA4-3687FEE00EE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07ED7936-D779-47E7-BF6C-7C086F04E976}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="67604082-326d-4240-aaee-100283b20839"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>